<commit_message>
Adds ability to select sheet name of the Excel file by its name.
</commit_message>
<xml_diff>
--- a/study02/test01.xlsx
+++ b/study02/test01.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\MounSinai\MoTrPac_API\ProgrammaticConnectivity\MountSinai_metadata_file_loader\study02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE79FE8-E293-49B7-85BC-BA80045D83F2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC34D2B-AC1A-42AD-AD8C-248CB5AEC723}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8B41012A-54BD-465D-9D80-AA2D8EC80760}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11265" xr2:uid="{8B41012A-54BD-465D-9D80-AA2D8EC80760}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="TestSheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>

</xml_diff>